<commit_message>
All project modifications applied (final version)
</commit_message>
<xml_diff>
--- a/data/real_data.xlsx
+++ b/data/real_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\PycharmProjects\MVCGUIGenerator\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\PycharmProjects\MVCGUIGenerator2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C63ECC-5C41-41D4-ADD7-79B24CF832EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32468F7B-F2B3-46A9-99B6-2BC5099A208E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="594" xr2:uid="{F8FC9E55-C964-41C2-BD90-4C178CD34650}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="594" xr2:uid="{F8FC9E55-C964-41C2-BD90-4C178CD34650}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1581" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="90">
   <si>
     <t/>
   </si>
@@ -206,180 +206,27 @@
     <t>Button</t>
   </si>
   <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>save</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>Controller</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
-    <t>getStudentName</t>
-  </si>
-  <si>
-    <t>setStudentName</t>
-  </si>
-  <si>
     <t>rollNo</t>
   </si>
   <si>
     <t>model.getName</t>
   </si>
   <si>
-    <t>setStudentRollNo</t>
-  </si>
-  <si>
     <t>model.getRollNo</t>
   </si>
   <si>
-    <t>getStudentRollNo</t>
-  </si>
-  <si>
     <t>StudentController</t>
   </si>
   <si>
-    <t>getBookTitle</t>
-  </si>
-  <si>
-    <t>BookController</t>
-  </si>
-  <si>
-    <t>setBookTitle</t>
-  </si>
-  <si>
-    <t>model.getTitle</t>
-  </si>
-  <si>
-    <t>setBookAuthor</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>getBookAuthor</t>
-  </si>
-  <si>
-    <t>model.getAuthor</t>
-  </si>
-  <si>
-    <t>author</t>
-  </si>
-  <si>
-    <t>getBookPrice</t>
-  </si>
-  <si>
-    <t>float</t>
-  </si>
-  <si>
-    <t>Spinbox</t>
-  </si>
-  <si>
-    <t>model.getPrice</t>
-  </si>
-  <si>
-    <t>setBookPrice</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
     <t>IsAReturnValue</t>
   </si>
   <si>
-    <t>getId</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>setId</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
-    <t>ClientController</t>
-  </si>
-  <si>
-    <t>model.getId</t>
-  </si>
-  <si>
-    <t>getName</t>
-  </si>
-  <si>
-    <t>setName</t>
-  </si>
-  <si>
-    <t>getSurname</t>
-  </si>
-  <si>
-    <t>model.getSurname</t>
-  </si>
-  <si>
-    <t>setSurname</t>
-  </si>
-  <si>
-    <t>surname</t>
-  </si>
-  <si>
-    <t>calculateCost</t>
-  </si>
-  <si>
-    <t>amount</t>
-  </si>
-  <si>
-    <t>gasType</t>
-  </si>
-  <si>
-    <t>GasPriceController</t>
-  </si>
-  <si>
-    <t>cost</t>
-  </si>
-  <si>
-    <t>list</t>
-  </si>
-  <si>
-    <t>noteController</t>
-  </si>
-  <si>
-    <t>Listbox</t>
-  </si>
-  <si>
-    <t>edit</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>result</t>
-  </si>
-  <si>
-    <t>noteObj.getNotes</t>
-  </si>
-  <si>
-    <t>noteObj.getNoteById</t>
-  </si>
-  <si>
-    <t>delete</t>
-  </si>
-  <si>
-    <t>bool</t>
-  </si>
-  <si>
-    <t>noteObj.deleteNoteById</t>
-  </si>
-  <si>
-    <t>Message</t>
-  </si>
-  <si>
     <t>PossibleValues</t>
   </si>
   <si>
@@ -387,6 +234,78 @@
   </si>
   <si>
     <t>UsedByView</t>
+  </si>
+  <si>
+    <t>add_task</t>
+  </si>
+  <si>
+    <t>set_student_name</t>
+  </si>
+  <si>
+    <t>model.get_name</t>
+  </si>
+  <si>
+    <t>get_student_name</t>
+  </si>
+  <si>
+    <t>roll_no</t>
+  </si>
+  <si>
+    <t>set_student_roll_no</t>
+  </si>
+  <si>
+    <t>model.get_roll_no</t>
+  </si>
+  <si>
+    <t>get_student_roll_no</t>
+  </si>
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <t>TaskController</t>
+  </si>
+  <si>
+    <t>set_person_name</t>
+  </si>
+  <si>
+    <t>PersonController</t>
+  </si>
+  <si>
+    <t>get_person_name</t>
+  </si>
+  <si>
+    <t>self.model.get_name</t>
+  </si>
+  <si>
+    <t>set_employee_name</t>
+  </si>
+  <si>
+    <t>EmployeeController</t>
+  </si>
+  <si>
+    <t>get_employee_name</t>
+  </si>
+  <si>
+    <t>set_employee_id</t>
+  </si>
+  <si>
+    <t>get_employee_id</t>
+  </si>
+  <si>
+    <t>self.model.get_id</t>
+  </si>
+  <si>
+    <t>set_employee_department</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>get_employee_department</t>
+  </si>
+  <si>
+    <t>self.model.get_department</t>
   </si>
 </sst>
 </file>
@@ -428,10 +347,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,66 +684,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CDEDF86-46A2-4A43-BB44-F65A93DE926D}">
-  <dimension ref="A1:BA48"/>
+  <dimension ref="A1:BA27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="AY1" sqref="AY1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" customWidth="1"/>
-    <col min="13" max="13" width="13.5546875" customWidth="1"/>
-    <col min="14" max="14" width="15" customWidth="1"/>
-    <col min="15" max="15" width="13.44140625" customWidth="1"/>
-    <col min="16" max="16" width="15" customWidth="1"/>
-    <col min="17" max="17" width="13.77734375" customWidth="1"/>
-    <col min="18" max="18" width="15" customWidth="1"/>
-    <col min="19" max="19" width="13.88671875" customWidth="1"/>
-    <col min="20" max="20" width="15" customWidth="1"/>
-    <col min="21" max="21" width="13.77734375" customWidth="1"/>
-    <col min="22" max="22" width="15" customWidth="1"/>
-    <col min="23" max="23" width="13.77734375" customWidth="1"/>
-    <col min="24" max="24" width="14.88671875" customWidth="1"/>
-    <col min="25" max="25" width="13.77734375" customWidth="1"/>
-    <col min="26" max="26" width="16.109375" customWidth="1"/>
-    <col min="27" max="27" width="14.88671875" customWidth="1"/>
-    <col min="28" max="28" width="22" customWidth="1"/>
-    <col min="29" max="29" width="16" customWidth="1"/>
-    <col min="30" max="30" width="17.109375" customWidth="1"/>
-    <col min="31" max="31" width="15.88671875" customWidth="1"/>
-    <col min="32" max="32" width="17" customWidth="1"/>
-    <col min="33" max="33" width="15.6640625" customWidth="1"/>
-    <col min="34" max="34" width="17.109375" customWidth="1"/>
-    <col min="35" max="35" width="16" customWidth="1"/>
-    <col min="36" max="36" width="17.21875" customWidth="1"/>
-    <col min="37" max="37" width="16.21875" customWidth="1"/>
-    <col min="38" max="38" width="17.44140625" customWidth="1"/>
-    <col min="39" max="39" width="16.33203125" customWidth="1"/>
-    <col min="40" max="40" width="17.33203125" customWidth="1"/>
-    <col min="41" max="41" width="16.109375" customWidth="1"/>
-    <col min="42" max="42" width="17.44140625" customWidth="1"/>
-    <col min="43" max="43" width="16" customWidth="1"/>
-    <col min="44" max="44" width="17.21875" customWidth="1"/>
-    <col min="45" max="45" width="15.88671875" customWidth="1"/>
-    <col min="46" max="46" width="18.21875" customWidth="1"/>
-    <col min="47" max="47" width="17.109375" customWidth="1"/>
-    <col min="49" max="49" width="13.77734375" customWidth="1"/>
-    <col min="50" max="50" width="17.88671875" customWidth="1"/>
-    <col min="51" max="51" width="17.6640625" customWidth="1"/>
-    <col min="52" max="52" width="15.77734375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" customWidth="1"/>
+    <col min="17" max="17" width="14.5703125" customWidth="1"/>
+    <col min="18" max="18" width="15.85546875" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" customWidth="1"/>
+    <col min="21" max="21" width="15.28515625" customWidth="1"/>
+    <col min="22" max="22" width="16.5703125" customWidth="1"/>
+    <col min="23" max="23" width="15.42578125" customWidth="1"/>
+    <col min="24" max="24" width="15.85546875" customWidth="1"/>
+    <col min="25" max="25" width="15" customWidth="1"/>
+    <col min="26" max="26" width="17.85546875" customWidth="1"/>
+    <col min="27" max="27" width="15.85546875" customWidth="1"/>
+    <col min="28" max="28" width="25" customWidth="1"/>
+    <col min="29" max="29" width="16.7109375" customWidth="1"/>
+    <col min="30" max="30" width="18.28515625" customWidth="1"/>
+    <col min="31" max="31" width="17.28515625" customWidth="1"/>
+    <col min="32" max="32" width="18.42578125" customWidth="1"/>
+    <col min="33" max="33" width="16.85546875" customWidth="1"/>
+    <col min="34" max="34" width="18.5703125" customWidth="1"/>
+    <col min="35" max="35" width="16.85546875" customWidth="1"/>
+    <col min="36" max="36" width="18" customWidth="1"/>
+    <col min="37" max="37" width="17.28515625" customWidth="1"/>
+    <col min="38" max="38" width="18.85546875" customWidth="1"/>
+    <col min="39" max="39" width="17.5703125" customWidth="1"/>
+    <col min="40" max="40" width="18.42578125" customWidth="1"/>
+    <col min="41" max="41" width="17.5703125" customWidth="1"/>
+    <col min="42" max="42" width="18.42578125" customWidth="1"/>
+    <col min="43" max="43" width="16.85546875" customWidth="1"/>
+    <col min="44" max="44" width="18.5703125" customWidth="1"/>
+    <col min="45" max="45" width="17" customWidth="1"/>
+    <col min="46" max="46" width="19.5703125" customWidth="1"/>
+    <col min="47" max="47" width="18.140625" customWidth="1"/>
+    <col min="48" max="48" width="14" customWidth="1"/>
+    <col min="49" max="49" width="13.7109375" customWidth="1"/>
+    <col min="50" max="50" width="25.7109375" customWidth="1"/>
+    <col min="51" max="51" width="17.7109375" customWidth="1"/>
+    <col min="52" max="52" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -845,7 +764,7 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -971,30 +890,30 @@
         <v>47</v>
       </c>
       <c r="AW1" t="s">
-        <v>114</v>
+        <v>63</v>
       </c>
       <c r="AX1" t="s">
         <v>48</v>
       </c>
-      <c r="AY1" s="2" t="s">
-        <v>115</v>
+      <c r="AY1" t="s">
+        <v>64</v>
       </c>
       <c r="AZ1" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="BA1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
         <v>49</v>
       </c>
       <c r="C2" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D2" s="1">
         <v>1.7976931348623101E+292</v>
@@ -1132,10 +1051,10 @@
         <v>0</v>
       </c>
       <c r="AX2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="AY2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="AZ2" t="s">
         <v>50</v>
@@ -1144,15 +1063,15 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D3" s="1">
         <v>1.7976931348623101E+292</v>
@@ -1167,7 +1086,7 @@
         <v>51</v>
       </c>
       <c r="H3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I3" t="s">
         <v>49</v>
@@ -1290,7 +1209,7 @@
         <v>0</v>
       </c>
       <c r="AY3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="AZ3" t="s">
         <v>50</v>
@@ -1299,15 +1218,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
         <v>49</v>
       </c>
       <c r="C4" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D4" s="1">
         <v>1.7976931348623101E+292</v>
@@ -1445,27 +1364,27 @@
         <v>0</v>
       </c>
       <c r="AX4" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="AY4" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="AZ4" t="s">
         <v>50</v>
       </c>
       <c r="BA4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
         <v>49</v>
       </c>
       <c r="C5" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D5" s="1">
         <v>1.7976931348623101E+292</v>
@@ -1540,7 +1459,7 @@
         <v>52</v>
       </c>
       <c r="AB5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AC5" t="s">
         <v>49</v>
@@ -1603,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="AY5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="AZ5" t="s">
         <v>50</v>
@@ -1612,15 +1531,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
         <v>49</v>
       </c>
       <c r="C6" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D6" s="1">
         <v>1.7976931348623101E+292</v>
@@ -1758,10 +1677,10 @@
         <v>0</v>
       </c>
       <c r="AX6" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="AY6" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="AZ6" t="s">
         <v>50</v>
@@ -1770,15 +1689,15 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>52</v>
       </c>
       <c r="C7" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D7" s="1">
         <v>1.7976931348623101E+292</v>
@@ -1793,7 +1712,7 @@
         <v>51</v>
       </c>
       <c r="H7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I7" t="s">
         <v>49</v>
@@ -1916,7 +1835,7 @@
         <v>0</v>
       </c>
       <c r="AY7" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="AZ7" t="s">
         <v>50</v>
@@ -1925,15 +1844,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
         <v>49</v>
       </c>
       <c r="C8" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D8" s="1">
         <v>1.7976931348623101E+292</v>
@@ -2071,27 +1990,27 @@
         <v>0</v>
       </c>
       <c r="AX8" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="AY8" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="AZ8" t="s">
         <v>50</v>
       </c>
       <c r="BA8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
         <v>49</v>
       </c>
       <c r="C9" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D9" s="1">
         <v>1.7976931348623101E+292</v>
@@ -2166,7 +2085,7 @@
         <v>52</v>
       </c>
       <c r="AB9" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="AC9" t="s">
         <v>49</v>
@@ -2229,7 +2148,7 @@
         <v>0</v>
       </c>
       <c r="AY9" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="AZ9" t="s">
         <v>50</v>
@@ -2238,15 +2157,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
         <v>52</v>
       </c>
       <c r="C10" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D10" s="1">
         <v>1.7976931348623101E+292</v>
@@ -2261,7 +2180,7 @@
         <v>51</v>
       </c>
       <c r="H10" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="I10" t="s">
         <v>49</v>
@@ -2324,7 +2243,7 @@
         <v>52</v>
       </c>
       <c r="AY10" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="AZ10" t="s">
         <v>50</v>
@@ -2333,15 +2252,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
         <v>49</v>
       </c>
       <c r="C11" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D11" s="1">
         <v>1.7976931348623101E+292</v>
@@ -2416,10 +2335,10 @@
         <v>52</v>
       </c>
       <c r="AX11" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="AY11" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="AZ11" t="s">
         <v>50</v>
@@ -2428,15 +2347,15 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C12" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D12" s="1">
         <v>1.7976931348623101E+292</v>
@@ -2450,8 +2369,11 @@
       <c r="G12" t="s">
         <v>51</v>
       </c>
+      <c r="H12" t="s">
+        <v>56</v>
+      </c>
       <c r="I12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="K12" t="s">
         <v>52</v>
@@ -2480,11 +2402,8 @@
       <c r="AA12" t="s">
         <v>52</v>
       </c>
-      <c r="AB12" t="s">
-        <v>72</v>
-      </c>
       <c r="AC12" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="AE12" t="s">
         <v>52</v>
@@ -2514,7 +2433,7 @@
         <v>52</v>
       </c>
       <c r="AY12" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="AZ12" t="s">
         <v>50</v>
@@ -2523,27 +2442,27 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
         <v>49</v>
       </c>
       <c r="C13" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D13" s="1">
         <v>1.7976931348623101E+292</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
         <v>51</v>
       </c>
       <c r="G13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I13" t="s">
         <v>52</v>
@@ -2606,27 +2525,27 @@
         <v>52</v>
       </c>
       <c r="AX13" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="AY13" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="AZ13" t="s">
         <v>50</v>
       </c>
       <c r="BA13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C14" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D14" s="1">
         <v>1.7976931348623101E+292</v>
@@ -2640,42 +2559,42 @@
       <c r="G14" t="s">
         <v>51</v>
       </c>
-      <c r="H14" t="s">
-        <v>74</v>
-      </c>
       <c r="I14" t="s">
+        <v>52</v>
+      </c>
+      <c r="K14" t="s">
+        <v>52</v>
+      </c>
+      <c r="M14" t="s">
+        <v>52</v>
+      </c>
+      <c r="O14" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>52</v>
+      </c>
+      <c r="S14" t="s">
+        <v>52</v>
+      </c>
+      <c r="U14" t="s">
+        <v>52</v>
+      </c>
+      <c r="W14" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC14" t="s">
         <v>49</v>
       </c>
-      <c r="K14" t="s">
-        <v>52</v>
-      </c>
-      <c r="M14" t="s">
-        <v>52</v>
-      </c>
-      <c r="O14" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>52</v>
-      </c>
-      <c r="S14" t="s">
-        <v>52</v>
-      </c>
-      <c r="U14" t="s">
-        <v>52</v>
-      </c>
-      <c r="W14" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>52</v>
-      </c>
       <c r="AE14" t="s">
         <v>52</v>
       </c>
@@ -2704,7 +2623,7 @@
         <v>52</v>
       </c>
       <c r="AY14" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="AZ14" t="s">
         <v>50</v>
@@ -2713,27 +2632,27 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
         <v>49</v>
       </c>
       <c r="C15" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D15" s="1">
         <v>1.7976931348623101E+292</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s">
         <v>51</v>
       </c>
       <c r="G15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I15" t="s">
         <v>52</v>
@@ -2796,10 +2715,10 @@
         <v>52</v>
       </c>
       <c r="AX15" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="AY15" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="AZ15" t="s">
         <v>50</v>
@@ -2808,15 +2727,15 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C16" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D16" s="1">
         <v>1.7976931348623101E+292</v>
@@ -2830,8 +2749,11 @@
       <c r="G16" t="s">
         <v>51</v>
       </c>
+      <c r="H16" t="s">
+        <v>56</v>
+      </c>
       <c r="I16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="K16" t="s">
         <v>52</v>
@@ -2860,11 +2782,8 @@
       <c r="AA16" t="s">
         <v>52</v>
       </c>
-      <c r="AB16" t="s">
-        <v>76</v>
-      </c>
       <c r="AC16" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="AE16" t="s">
         <v>52</v>
@@ -2894,7 +2813,7 @@
         <v>52</v>
       </c>
       <c r="AY16" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="AZ16" t="s">
         <v>50</v>
@@ -2903,27 +2822,27 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
         <v>49</v>
       </c>
       <c r="C17" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D17" s="1">
         <v>1.7976931348623101E+292</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F17" t="s">
         <v>51</v>
       </c>
       <c r="G17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I17" t="s">
         <v>52</v>
@@ -2986,27 +2905,27 @@
         <v>52</v>
       </c>
       <c r="AX17" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="AY17" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="AZ17" t="s">
         <v>50</v>
       </c>
       <c r="BA17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C18" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D18" s="1">
         <v>1.7976931348623101E+292</v>
@@ -3020,42 +2939,42 @@
       <c r="G18" t="s">
         <v>51</v>
       </c>
-      <c r="H18" t="s">
-        <v>77</v>
-      </c>
       <c r="I18" t="s">
+        <v>52</v>
+      </c>
+      <c r="K18" t="s">
+        <v>52</v>
+      </c>
+      <c r="M18" t="s">
+        <v>52</v>
+      </c>
+      <c r="O18" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>52</v>
+      </c>
+      <c r="S18" t="s">
+        <v>52</v>
+      </c>
+      <c r="U18" t="s">
+        <v>52</v>
+      </c>
+      <c r="W18" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC18" t="s">
         <v>49</v>
       </c>
-      <c r="K18" t="s">
-        <v>52</v>
-      </c>
-      <c r="M18" t="s">
-        <v>52</v>
-      </c>
-      <c r="O18" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>52</v>
-      </c>
-      <c r="S18" t="s">
-        <v>52</v>
-      </c>
-      <c r="U18" t="s">
-        <v>52</v>
-      </c>
-      <c r="W18" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>52</v>
-      </c>
       <c r="AE18" t="s">
         <v>52</v>
       </c>
@@ -3084,7 +3003,7 @@
         <v>52</v>
       </c>
       <c r="AY18" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="AZ18" t="s">
         <v>50</v>
@@ -3093,27 +3012,27 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
         <v>49</v>
       </c>
       <c r="C19" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D19" s="1">
         <v>1.7976931348623101E+292</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F19" t="s">
         <v>51</v>
       </c>
       <c r="G19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I19" t="s">
         <v>52</v>
@@ -3176,10 +3095,10 @@
         <v>52</v>
       </c>
       <c r="AX19" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="AY19" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="AZ19" t="s">
         <v>50</v>
@@ -3188,15 +3107,15 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="C20" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D20" s="1">
         <v>1.7976931348623101E+292</v>
@@ -3210,8 +3129,11 @@
       <c r="G20" t="s">
         <v>51</v>
       </c>
+      <c r="H20" t="s">
+        <v>62</v>
+      </c>
       <c r="I20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="K20" t="s">
         <v>52</v>
@@ -3240,41 +3162,38 @@
       <c r="AA20" t="s">
         <v>52</v>
       </c>
-      <c r="AB20" t="s">
+      <c r="AC20" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM20" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO20" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ20" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS20" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU20" t="s">
+        <v>52</v>
+      </c>
+      <c r="AY20" t="s">
         <v>81</v>
-      </c>
-      <c r="AC20" t="s">
-        <v>79</v>
-      </c>
-      <c r="AE20" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG20" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI20" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK20" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM20" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO20" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ20" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS20" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU20" t="s">
-        <v>52</v>
-      </c>
-      <c r="AY20" t="s">
-        <v>70</v>
       </c>
       <c r="AZ20" t="s">
         <v>50</v>
@@ -3283,27 +3202,27 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="C21" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D21" s="1">
         <v>1.7976931348623101E+292</v>
       </c>
       <c r="E21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F21" t="s">
         <v>51</v>
       </c>
       <c r="G21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I21" t="s">
         <v>52</v>
@@ -3366,27 +3285,27 @@
         <v>52</v>
       </c>
       <c r="AX21" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="AY21" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="AZ21" t="s">
         <v>50</v>
       </c>
       <c r="BA21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C22" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D22" s="1">
         <v>1.7976931348623101E+292</v>
@@ -3400,11 +3319,8 @@
       <c r="G22" t="s">
         <v>51</v>
       </c>
-      <c r="H22" t="s">
-        <v>83</v>
-      </c>
       <c r="I22" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="K22" t="s">
         <v>52</v>
@@ -3433,8 +3349,11 @@
       <c r="AA22" t="s">
         <v>52</v>
       </c>
+      <c r="AB22" t="s">
+        <v>85</v>
+      </c>
       <c r="AC22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AE22" t="s">
         <v>52</v>
@@ -3464,7 +3383,7 @@
         <v>52</v>
       </c>
       <c r="AY22" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="AZ22" t="s">
         <v>50</v>
@@ -3473,27 +3392,27 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="C23" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D23" s="1">
         <v>1.7976931348623101E+292</v>
       </c>
       <c r="E23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F23" t="s">
         <v>51</v>
       </c>
       <c r="G23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I23" t="s">
         <v>52</v>
@@ -3556,27 +3475,27 @@
         <v>52</v>
       </c>
       <c r="AX23" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AY23" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="AZ23" t="s">
         <v>50</v>
       </c>
       <c r="BA23" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="C24" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D24" s="1">
         <v>1.7976931348623101E+292</v>
@@ -3590,8 +3509,11 @@
       <c r="G24" t="s">
         <v>51</v>
       </c>
+      <c r="H24" t="s">
+        <v>87</v>
+      </c>
       <c r="I24" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="K24" t="s">
         <v>52</v>
@@ -3620,11 +3542,8 @@
       <c r="AA24" t="s">
         <v>52</v>
       </c>
-      <c r="AB24" t="s">
-        <v>90</v>
-      </c>
       <c r="AC24" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="AE24" t="s">
         <v>52</v>
@@ -3654,7 +3573,7 @@
         <v>52</v>
       </c>
       <c r="AY24" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="AZ24" t="s">
         <v>50</v>
@@ -3663,27 +3582,27 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="C25" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D25" s="1">
         <v>1.7976931348623101E+292</v>
       </c>
       <c r="E25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F25" t="s">
         <v>51</v>
       </c>
       <c r="G25" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I25" t="s">
         <v>52</v>
@@ -3746,27 +3665,27 @@
         <v>52</v>
       </c>
       <c r="AX25" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AY25" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="AZ25" t="s">
         <v>50</v>
       </c>
       <c r="BA25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C26" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D26" s="1">
         <v>1.7976931348623101E+292</v>
@@ -3780,11 +3699,8 @@
       <c r="G26" t="s">
         <v>51</v>
       </c>
-      <c r="H26" t="s">
-        <v>88</v>
-      </c>
       <c r="I26" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="K26" t="s">
         <v>52</v>
@@ -3813,8 +3729,11 @@
       <c r="AA26" t="s">
         <v>52</v>
       </c>
+      <c r="AB26" t="s">
+        <v>89</v>
+      </c>
       <c r="AC26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AE26" t="s">
         <v>52</v>
@@ -3844,7 +3763,7 @@
         <v>52</v>
       </c>
       <c r="AY26" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="AZ26" t="s">
         <v>50</v>
@@ -3853,27 +3772,27 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="C27" s="1">
-        <v>2.2250738585072E-292</v>
+        <v>-1.7976931348623101E+292</v>
       </c>
       <c r="D27" s="1">
         <v>1.7976931348623101E+292</v>
       </c>
       <c r="E27" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F27" t="s">
         <v>51</v>
       </c>
       <c r="G27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I27" t="s">
         <v>52</v>
@@ -3936,2014 +3855,16 @@
         <v>52</v>
       </c>
       <c r="AX27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AY27" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="AZ27" t="s">
         <v>50</v>
       </c>
       <c r="BA27" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>91</v>
-      </c>
-      <c r="B28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E28" t="s">
-        <v>51</v>
-      </c>
-      <c r="F28" t="s">
-        <v>50</v>
-      </c>
-      <c r="G28" t="s">
-        <v>51</v>
-      </c>
-      <c r="I28" t="s">
-        <v>52</v>
-      </c>
-      <c r="K28" t="s">
-        <v>52</v>
-      </c>
-      <c r="M28" t="s">
-        <v>52</v>
-      </c>
-      <c r="O28" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>52</v>
-      </c>
-      <c r="S28" t="s">
-        <v>52</v>
-      </c>
-      <c r="U28" t="s">
-        <v>52</v>
-      </c>
-      <c r="W28" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA28" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC28" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE28" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG28" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI28" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK28" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM28" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO28" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ28" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS28" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU28" t="s">
-        <v>52</v>
-      </c>
-      <c r="AY28" t="s">
-        <v>89</v>
-      </c>
-      <c r="AZ28" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E29" t="s">
-        <v>51</v>
-      </c>
-      <c r="F29" t="s">
-        <v>51</v>
-      </c>
-      <c r="G29" t="s">
-        <v>50</v>
-      </c>
-      <c r="I29" t="s">
-        <v>52</v>
-      </c>
-      <c r="K29" t="s">
-        <v>52</v>
-      </c>
-      <c r="M29" t="s">
-        <v>52</v>
-      </c>
-      <c r="O29" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>52</v>
-      </c>
-      <c r="S29" t="s">
-        <v>52</v>
-      </c>
-      <c r="U29" t="s">
-        <v>52</v>
-      </c>
-      <c r="W29" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA29" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC29" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE29" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG29" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI29" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK29" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM29" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO29" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ29" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS29" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU29" t="s">
-        <v>52</v>
-      </c>
-      <c r="AX29" t="s">
-        <v>91</v>
-      </c>
-      <c r="AY29" t="s">
-        <v>89</v>
-      </c>
-      <c r="AZ29" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>92</v>
-      </c>
-      <c r="B30" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D30" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E30" t="s">
-        <v>51</v>
-      </c>
-      <c r="F30" t="s">
-        <v>50</v>
-      </c>
-      <c r="G30" t="s">
-        <v>51</v>
-      </c>
-      <c r="H30" t="s">
-        <v>60</v>
-      </c>
-      <c r="I30" t="s">
-        <v>49</v>
-      </c>
-      <c r="K30" t="s">
-        <v>52</v>
-      </c>
-      <c r="M30" t="s">
-        <v>52</v>
-      </c>
-      <c r="O30" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>52</v>
-      </c>
-      <c r="S30" t="s">
-        <v>52</v>
-      </c>
-      <c r="U30" t="s">
-        <v>52</v>
-      </c>
-      <c r="W30" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y30" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA30" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC30" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE30" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG30" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI30" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK30" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM30" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO30" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ30" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS30" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU30" t="s">
-        <v>52</v>
-      </c>
-      <c r="AY30" t="s">
-        <v>89</v>
-      </c>
-      <c r="AZ30" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA30" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>60</v>
-      </c>
-      <c r="B31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D31" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E31" t="s">
-        <v>50</v>
-      </c>
-      <c r="F31" t="s">
-        <v>51</v>
-      </c>
-      <c r="G31" t="s">
-        <v>51</v>
-      </c>
-      <c r="I31" t="s">
-        <v>52</v>
-      </c>
-      <c r="K31" t="s">
-        <v>52</v>
-      </c>
-      <c r="M31" t="s">
-        <v>52</v>
-      </c>
-      <c r="O31" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>52</v>
-      </c>
-      <c r="S31" t="s">
-        <v>52</v>
-      </c>
-      <c r="U31" t="s">
-        <v>52</v>
-      </c>
-      <c r="W31" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y31" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA31" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC31" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE31" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG31" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI31" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK31" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM31" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO31" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ31" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS31" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU31" t="s">
-        <v>52</v>
-      </c>
-      <c r="AX31" t="s">
-        <v>92</v>
-      </c>
-      <c r="AY31" t="s">
-        <v>89</v>
-      </c>
-      <c r="AZ31" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>93</v>
-      </c>
-      <c r="B32" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D32" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E32" t="s">
-        <v>51</v>
-      </c>
-      <c r="F32" t="s">
-        <v>50</v>
-      </c>
-      <c r="G32" t="s">
-        <v>51</v>
-      </c>
-      <c r="I32" t="s">
-        <v>52</v>
-      </c>
-      <c r="K32" t="s">
-        <v>52</v>
-      </c>
-      <c r="M32" t="s">
-        <v>52</v>
-      </c>
-      <c r="O32" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S32" t="s">
-        <v>52</v>
-      </c>
-      <c r="U32" t="s">
-        <v>52</v>
-      </c>
-      <c r="W32" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y32" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA32" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC32" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE32" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG32" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI32" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK32" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM32" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO32" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ32" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS32" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU32" t="s">
-        <v>52</v>
-      </c>
-      <c r="AY32" t="s">
-        <v>89</v>
-      </c>
-      <c r="AZ32" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA32" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>94</v>
-      </c>
-      <c r="B33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E33" t="s">
-        <v>51</v>
-      </c>
-      <c r="F33" t="s">
-        <v>51</v>
-      </c>
-      <c r="G33" t="s">
-        <v>50</v>
-      </c>
-      <c r="I33" t="s">
-        <v>52</v>
-      </c>
-      <c r="K33" t="s">
-        <v>52</v>
-      </c>
-      <c r="M33" t="s">
-        <v>52</v>
-      </c>
-      <c r="O33" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>52</v>
-      </c>
-      <c r="S33" t="s">
-        <v>52</v>
-      </c>
-      <c r="U33" t="s">
-        <v>52</v>
-      </c>
-      <c r="W33" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y33" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA33" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC33" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE33" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG33" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI33" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK33" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM33" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO33" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ33" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS33" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU33" t="s">
-        <v>52</v>
-      </c>
-      <c r="AX33" t="s">
-        <v>93</v>
-      </c>
-      <c r="AY33" t="s">
-        <v>89</v>
-      </c>
-      <c r="AZ33" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>95</v>
-      </c>
-      <c r="B34" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D34" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E34" t="s">
-        <v>51</v>
-      </c>
-      <c r="F34" t="s">
-        <v>50</v>
-      </c>
-      <c r="G34" t="s">
-        <v>51</v>
-      </c>
-      <c r="H34" t="s">
-        <v>96</v>
-      </c>
-      <c r="I34" t="s">
-        <v>49</v>
-      </c>
-      <c r="K34" t="s">
-        <v>52</v>
-      </c>
-      <c r="M34" t="s">
-        <v>52</v>
-      </c>
-      <c r="O34" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>52</v>
-      </c>
-      <c r="S34" t="s">
-        <v>52</v>
-      </c>
-      <c r="U34" t="s">
-        <v>52</v>
-      </c>
-      <c r="W34" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y34" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA34" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC34" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE34" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG34" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI34" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK34" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM34" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO34" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ34" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS34" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU34" t="s">
-        <v>52</v>
-      </c>
-      <c r="AY34" t="s">
-        <v>89</v>
-      </c>
-      <c r="AZ34" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA34" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>96</v>
-      </c>
-      <c r="B35" t="s">
-        <v>49</v>
-      </c>
-      <c r="C35" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D35" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E35" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" t="s">
-        <v>51</v>
-      </c>
-      <c r="G35" t="s">
-        <v>51</v>
-      </c>
-      <c r="I35" t="s">
-        <v>52</v>
-      </c>
-      <c r="K35" t="s">
-        <v>52</v>
-      </c>
-      <c r="M35" t="s">
-        <v>52</v>
-      </c>
-      <c r="O35" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>52</v>
-      </c>
-      <c r="S35" t="s">
-        <v>52</v>
-      </c>
-      <c r="U35" t="s">
-        <v>52</v>
-      </c>
-      <c r="W35" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y35" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA35" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC35" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE35" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG35" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI35" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK35" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM35" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO35" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ35" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS35" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU35" t="s">
-        <v>52</v>
-      </c>
-      <c r="AX35" t="s">
-        <v>95</v>
-      </c>
-      <c r="AY35" t="s">
-        <v>89</v>
-      </c>
-      <c r="AZ35" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA35" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>97</v>
-      </c>
-      <c r="B36" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D36" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E36" t="s">
-        <v>51</v>
-      </c>
-      <c r="F36" t="s">
-        <v>50</v>
-      </c>
-      <c r="G36" t="s">
-        <v>51</v>
-      </c>
-      <c r="H36" t="s">
-        <v>98</v>
-      </c>
-      <c r="I36" t="s">
-        <v>79</v>
-      </c>
-      <c r="J36" t="s">
-        <v>99</v>
-      </c>
-      <c r="K36" t="s">
-        <v>49</v>
-      </c>
-      <c r="M36" t="s">
-        <v>52</v>
-      </c>
-      <c r="O36" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>52</v>
-      </c>
-      <c r="S36" t="s">
-        <v>52</v>
-      </c>
-      <c r="U36" t="s">
-        <v>52</v>
-      </c>
-      <c r="W36" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y36" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA36" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB36" t="s">
-        <v>101</v>
-      </c>
-      <c r="AC36" t="s">
-        <v>79</v>
-      </c>
-      <c r="AE36" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG36" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI36" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK36" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM36" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO36" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ36" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS36" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU36" t="s">
-        <v>52</v>
-      </c>
-      <c r="AY36" t="s">
-        <v>100</v>
-      </c>
-      <c r="AZ36" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA36" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>98</v>
-      </c>
-      <c r="B37" t="s">
-        <v>79</v>
-      </c>
-      <c r="C37" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D37" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E37" t="s">
-        <v>50</v>
-      </c>
-      <c r="F37" t="s">
-        <v>51</v>
-      </c>
-      <c r="G37" t="s">
-        <v>51</v>
-      </c>
-      <c r="I37" t="s">
-        <v>52</v>
-      </c>
-      <c r="K37" t="s">
-        <v>52</v>
-      </c>
-      <c r="M37" t="s">
-        <v>52</v>
-      </c>
-      <c r="O37" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>52</v>
-      </c>
-      <c r="S37" t="s">
-        <v>52</v>
-      </c>
-      <c r="U37" t="s">
-        <v>52</v>
-      </c>
-      <c r="W37" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y37" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA37" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC37" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE37" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG37" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI37" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK37" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM37" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO37" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ37" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS37" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU37" t="s">
-        <v>52</v>
-      </c>
-      <c r="AX37" t="s">
-        <v>97</v>
-      </c>
-      <c r="AY37" t="s">
-        <v>100</v>
-      </c>
-      <c r="AZ37" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA37" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>99</v>
-      </c>
-      <c r="B38" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D38" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E38" t="s">
-        <v>50</v>
-      </c>
-      <c r="F38" t="s">
-        <v>51</v>
-      </c>
-      <c r="G38" t="s">
-        <v>51</v>
-      </c>
-      <c r="I38" t="s">
-        <v>52</v>
-      </c>
-      <c r="K38" t="s">
-        <v>52</v>
-      </c>
-      <c r="M38" t="s">
-        <v>52</v>
-      </c>
-      <c r="O38" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>52</v>
-      </c>
-      <c r="S38" t="s">
-        <v>52</v>
-      </c>
-      <c r="U38" t="s">
-        <v>52</v>
-      </c>
-      <c r="W38" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y38" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA38" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC38" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE38" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG38" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI38" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK38" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM38" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO38" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ38" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS38" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU38" t="s">
-        <v>52</v>
-      </c>
-      <c r="AX38" t="s">
-        <v>97</v>
-      </c>
-      <c r="AY38" t="s">
-        <v>100</v>
-      </c>
-      <c r="AZ38" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA38" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>101</v>
-      </c>
-      <c r="B39" t="s">
-        <v>79</v>
-      </c>
-      <c r="C39" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D39" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E39" t="s">
-        <v>51</v>
-      </c>
-      <c r="F39" t="s">
-        <v>51</v>
-      </c>
-      <c r="G39" t="s">
-        <v>50</v>
-      </c>
-      <c r="I39" t="s">
-        <v>52</v>
-      </c>
-      <c r="K39" t="s">
-        <v>52</v>
-      </c>
-      <c r="M39" t="s">
-        <v>52</v>
-      </c>
-      <c r="O39" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>52</v>
-      </c>
-      <c r="S39" t="s">
-        <v>52</v>
-      </c>
-      <c r="U39" t="s">
-        <v>52</v>
-      </c>
-      <c r="W39" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y39" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA39" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC39" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE39" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG39" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI39" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK39" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM39" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO39" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ39" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS39" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU39" t="s">
-        <v>52</v>
-      </c>
-      <c r="AX39" t="s">
-        <v>97</v>
-      </c>
-      <c r="AY39" t="s">
-        <v>100</v>
-      </c>
-      <c r="AZ39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA39" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>102</v>
-      </c>
-      <c r="B40" t="s">
-        <v>102</v>
-      </c>
-      <c r="C40" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D40" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E40" t="s">
-        <v>51</v>
-      </c>
-      <c r="F40" t="s">
-        <v>50</v>
-      </c>
-      <c r="G40" t="s">
-        <v>51</v>
-      </c>
-      <c r="I40" t="s">
-        <v>52</v>
-      </c>
-      <c r="K40" t="s">
-        <v>52</v>
-      </c>
-      <c r="M40" t="s">
-        <v>52</v>
-      </c>
-      <c r="O40" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>52</v>
-      </c>
-      <c r="S40" t="s">
-        <v>52</v>
-      </c>
-      <c r="U40" t="s">
-        <v>52</v>
-      </c>
-      <c r="W40" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y40" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA40" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB40" t="s">
-        <v>108</v>
-      </c>
-      <c r="AC40" t="s">
-        <v>102</v>
-      </c>
-      <c r="AE40" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG40" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI40" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK40" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM40" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO40" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ40" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS40" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU40" t="s">
-        <v>52</v>
-      </c>
-      <c r="AY40" t="s">
-        <v>103</v>
-      </c>
-      <c r="AZ40" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA40" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>108</v>
-      </c>
-      <c r="B41" t="s">
-        <v>102</v>
-      </c>
-      <c r="C41" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D41" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E41" t="s">
-        <v>51</v>
-      </c>
-      <c r="F41" t="s">
-        <v>51</v>
-      </c>
-      <c r="G41" t="s">
-        <v>50</v>
-      </c>
-      <c r="I41" t="s">
-        <v>52</v>
-      </c>
-      <c r="K41" t="s">
-        <v>52</v>
-      </c>
-      <c r="M41" t="s">
-        <v>52</v>
-      </c>
-      <c r="O41" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>52</v>
-      </c>
-      <c r="S41" t="s">
-        <v>52</v>
-      </c>
-      <c r="U41" t="s">
-        <v>52</v>
-      </c>
-      <c r="W41" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y41" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA41" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC41" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE41" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG41" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI41" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK41" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM41" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO41" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ41" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS41" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU41" t="s">
-        <v>52</v>
-      </c>
-      <c r="AX41" t="s">
-        <v>102</v>
-      </c>
-      <c r="AY41" t="s">
-        <v>103</v>
-      </c>
-      <c r="AZ41" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA41" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>105</v>
-      </c>
-      <c r="B42" t="s">
-        <v>49</v>
-      </c>
-      <c r="C42" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D42" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E42" t="s">
-        <v>51</v>
-      </c>
-      <c r="F42" t="s">
-        <v>50</v>
-      </c>
-      <c r="G42" t="s">
-        <v>51</v>
-      </c>
-      <c r="H42" t="s">
-        <v>88</v>
-      </c>
-      <c r="I42" t="s">
-        <v>49</v>
-      </c>
-      <c r="K42" t="s">
-        <v>52</v>
-      </c>
-      <c r="M42" t="s">
-        <v>52</v>
-      </c>
-      <c r="O42" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>52</v>
-      </c>
-      <c r="S42" t="s">
-        <v>52</v>
-      </c>
-      <c r="U42" t="s">
-        <v>52</v>
-      </c>
-      <c r="W42" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y42" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA42" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB42" t="s">
-        <v>109</v>
-      </c>
-      <c r="AC42" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE42" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG42" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI42" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK42" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM42" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO42" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ42" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS42" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU42" t="s">
-        <v>52</v>
-      </c>
-      <c r="AY42" t="s">
-        <v>103</v>
-      </c>
-      <c r="AZ42" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA42" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>88</v>
-      </c>
-      <c r="B43" t="s">
-        <v>49</v>
-      </c>
-      <c r="C43" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D43" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E43" t="s">
-        <v>50</v>
-      </c>
-      <c r="F43" t="s">
-        <v>51</v>
-      </c>
-      <c r="G43" t="s">
-        <v>51</v>
-      </c>
-      <c r="I43" t="s">
-        <v>52</v>
-      </c>
-      <c r="K43" t="s">
-        <v>52</v>
-      </c>
-      <c r="M43" t="s">
-        <v>52</v>
-      </c>
-      <c r="O43" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>52</v>
-      </c>
-      <c r="S43" t="s">
-        <v>52</v>
-      </c>
-      <c r="U43" t="s">
-        <v>52</v>
-      </c>
-      <c r="W43" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y43" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA43" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC43" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE43" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG43" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI43" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK43" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM43" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO43" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ43" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS43" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU43" t="s">
-        <v>52</v>
-      </c>
-      <c r="AX43" t="s">
-        <v>105</v>
-      </c>
-      <c r="AY43" t="s">
-        <v>103</v>
-      </c>
-      <c r="AZ43" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA43" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="44" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>109</v>
-      </c>
-      <c r="B44" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D44" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E44" t="s">
-        <v>51</v>
-      </c>
-      <c r="F44" t="s">
-        <v>51</v>
-      </c>
-      <c r="G44" t="s">
-        <v>50</v>
-      </c>
-      <c r="I44" t="s">
-        <v>52</v>
-      </c>
-      <c r="K44" t="s">
-        <v>52</v>
-      </c>
-      <c r="M44" t="s">
-        <v>52</v>
-      </c>
-      <c r="O44" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>52</v>
-      </c>
-      <c r="S44" t="s">
-        <v>52</v>
-      </c>
-      <c r="U44" t="s">
-        <v>52</v>
-      </c>
-      <c r="W44" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y44" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA44" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC44" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE44" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG44" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI44" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK44" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM44" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO44" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ44" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS44" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU44" t="s">
-        <v>52</v>
-      </c>
-      <c r="AX44" t="s">
-        <v>105</v>
-      </c>
-      <c r="AY44" t="s">
-        <v>103</v>
-      </c>
-      <c r="AZ44" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA44" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>57</v>
-      </c>
-      <c r="B45" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D45" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E45" t="s">
-        <v>51</v>
-      </c>
-      <c r="F45" t="s">
-        <v>50</v>
-      </c>
-      <c r="G45" t="s">
-        <v>51</v>
-      </c>
-      <c r="I45" t="s">
-        <v>52</v>
-      </c>
-      <c r="K45" t="s">
-        <v>52</v>
-      </c>
-      <c r="M45" t="s">
-        <v>52</v>
-      </c>
-      <c r="O45" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>52</v>
-      </c>
-      <c r="S45" t="s">
-        <v>52</v>
-      </c>
-      <c r="U45" t="s">
-        <v>52</v>
-      </c>
-      <c r="W45" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y45" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA45" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB45" t="s">
-        <v>107</v>
-      </c>
-      <c r="AC45" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE45" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG45" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI45" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK45" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM45" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO45" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ45" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS45" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU45" t="s">
-        <v>52</v>
-      </c>
-      <c r="AY45" t="s">
-        <v>103</v>
-      </c>
-      <c r="AZ45" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA45" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>107</v>
-      </c>
-      <c r="B46" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D46" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E46" t="s">
-        <v>51</v>
-      </c>
-      <c r="F46" t="s">
-        <v>51</v>
-      </c>
-      <c r="G46" t="s">
-        <v>50</v>
-      </c>
-      <c r="I46" t="s">
-        <v>52</v>
-      </c>
-      <c r="K46" t="s">
-        <v>52</v>
-      </c>
-      <c r="M46" t="s">
-        <v>52</v>
-      </c>
-      <c r="O46" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>52</v>
-      </c>
-      <c r="S46" t="s">
-        <v>52</v>
-      </c>
-      <c r="U46" t="s">
-        <v>52</v>
-      </c>
-      <c r="W46" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y46" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA46" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC46" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE46" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG46" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI46" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK46" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM46" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO46" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ46" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS46" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU46" t="s">
-        <v>52</v>
-      </c>
-      <c r="AX46" t="s">
-        <v>57</v>
-      </c>
-      <c r="AY46" t="s">
-        <v>103</v>
-      </c>
-      <c r="AZ46" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA46" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="47" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>110</v>
-      </c>
-      <c r="B47" t="s">
-        <v>111</v>
-      </c>
-      <c r="C47" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E47" t="s">
-        <v>51</v>
-      </c>
-      <c r="F47" t="s">
-        <v>50</v>
-      </c>
-      <c r="G47" t="s">
-        <v>51</v>
-      </c>
-      <c r="I47" t="s">
-        <v>52</v>
-      </c>
-      <c r="K47" t="s">
-        <v>52</v>
-      </c>
-      <c r="M47" t="s">
-        <v>52</v>
-      </c>
-      <c r="O47" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>52</v>
-      </c>
-      <c r="S47" t="s">
-        <v>52</v>
-      </c>
-      <c r="U47" t="s">
-        <v>52</v>
-      </c>
-      <c r="W47" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y47" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA47" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB47" t="s">
-        <v>112</v>
-      </c>
-      <c r="AC47" t="s">
-        <v>111</v>
-      </c>
-      <c r="AE47" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG47" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI47" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK47" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM47" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO47" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ47" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS47" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU47" t="s">
-        <v>52</v>
-      </c>
-      <c r="AY47" t="s">
-        <v>103</v>
-      </c>
-      <c r="AZ47" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA47" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="48" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>112</v>
-      </c>
-      <c r="B48" t="s">
-        <v>111</v>
-      </c>
-      <c r="C48" s="1">
-        <v>2.2250738585072E-292</v>
-      </c>
-      <c r="D48" s="1">
-        <v>1.7976931348623101E+292</v>
-      </c>
-      <c r="E48" t="s">
-        <v>51</v>
-      </c>
-      <c r="F48" t="s">
-        <v>51</v>
-      </c>
-      <c r="G48" t="s">
-        <v>50</v>
-      </c>
-      <c r="I48" t="s">
-        <v>52</v>
-      </c>
-      <c r="K48" t="s">
-        <v>52</v>
-      </c>
-      <c r="M48" t="s">
-        <v>52</v>
-      </c>
-      <c r="O48" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>52</v>
-      </c>
-      <c r="S48" t="s">
-        <v>52</v>
-      </c>
-      <c r="U48" t="s">
-        <v>52</v>
-      </c>
-      <c r="W48" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y48" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA48" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC48" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE48" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG48" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI48" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK48" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM48" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO48" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ48" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS48" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU48" t="s">
-        <v>52</v>
-      </c>
-      <c r="AX48" t="s">
-        <v>110</v>
-      </c>
-      <c r="AY48" t="s">
-        <v>103</v>
-      </c>
-      <c r="AZ48" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA48" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>